<commit_message>
updated 2nd hand data
</commit_message>
<xml_diff>
--- a/Data4Dipesh/2hand Data_Final.xlsx
+++ b/Data4Dipesh/2hand Data_Final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/more/Desktop/Data4Dipesh/2hand Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81AF4583-8A4B-B44E-82CC-2A66AF0BB108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F1E367E-0F78-F640-B8BA-AE81852E70F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{E91E4898-FD52-D146-A301-D679369FD159}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{E91E4898-FD52-D146-A301-D679369FD159}"/>
   </bookViews>
   <sheets>
     <sheet name="Red Oak" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="28">
   <si>
     <t>Temperature/℃</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>360-min</t>
+  </si>
+  <si>
+    <t>delta_E</t>
   </si>
 </sst>
 </file>
@@ -503,10 +506,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CDB967C-A156-214C-B511-A1FE124FEFF7}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -517,7 +520,7 @@
     <col min="4" max="9" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>7</v>
       </c>
@@ -545,8 +548,11 @@
       <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J1" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
@@ -574,8 +580,12 @@
       <c r="I2" s="7">
         <v>24.09</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J2" s="1">
+        <f>SQRT((D2-G2)^2+(E2-H2)^2+(F2-I2)^2)</f>
+        <v>2.5665930725379913</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
@@ -603,8 +613,12 @@
       <c r="I3" s="3">
         <v>22.99</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J3" s="1">
+        <f t="shared" ref="J3:J22" si="0">SQRT((D3-G3)^2+(E3-H3)^2+(F3-I3)^2)</f>
+        <v>4.6909060958411901</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
@@ -632,8 +646,12 @@
       <c r="I4" s="3">
         <v>24.24</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J4" s="1">
+        <f t="shared" si="0"/>
+        <v>6.6966036167597727</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
@@ -661,8 +679,12 @@
       <c r="I5" s="3">
         <v>20.399999999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J5" s="1">
+        <f t="shared" si="0"/>
+        <v>12.804686642007296</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
@@ -690,8 +712,12 @@
       <c r="I6" s="3">
         <v>18.7</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J6" s="1">
+        <f t="shared" si="0"/>
+        <v>19.151501246638606</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>10</v>
       </c>
@@ -719,8 +745,12 @@
       <c r="I7" s="3">
         <v>17.600000000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J7" s="1">
+        <f t="shared" si="0"/>
+        <v>21.581705215297514</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -748,8 +778,12 @@
       <c r="I8" s="3">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J8" s="1">
+        <f t="shared" si="0"/>
+        <v>26.918580943281544</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>10</v>
       </c>
@@ -777,8 +811,12 @@
       <c r="I9" s="3">
         <v>15.7</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J9" s="1">
+        <f t="shared" si="0"/>
+        <v>26.92860932168611</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>10</v>
       </c>
@@ -806,8 +844,12 @@
       <c r="I10" s="3">
         <v>13.5</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J10" s="1">
+        <f t="shared" si="0"/>
+        <v>31.351395503230794</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
@@ -835,8 +877,12 @@
       <c r="I11" s="3">
         <v>8.8000000000000007</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J11" s="1">
+        <f t="shared" si="0"/>
+        <v>39.165801408882217</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>10</v>
       </c>
@@ -864,8 +910,12 @@
       <c r="I12" s="3">
         <v>7.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J12" s="1">
+        <f t="shared" si="0"/>
+        <v>42.533516196054144</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>10</v>
       </c>
@@ -893,8 +943,12 @@
       <c r="I13" s="3">
         <v>7.5</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J13" s="1">
+        <f t="shared" si="0"/>
+        <v>43.193286515383384</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>11</v>
       </c>
@@ -922,8 +976,12 @@
       <c r="I14" s="8">
         <v>20.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J14" s="1">
+        <f t="shared" si="0"/>
+        <v>11.427160627207446</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>11</v>
       </c>
@@ -951,8 +1009,12 @@
       <c r="I15" s="8">
         <v>20.5</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J15" s="1">
+        <f t="shared" si="0"/>
+        <v>9.2010868923187612</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>11</v>
       </c>
@@ -980,8 +1042,12 @@
       <c r="I16" s="8">
         <v>20.7</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J16" s="1">
+        <f t="shared" si="0"/>
+        <v>8.3815273071201055</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>11</v>
       </c>
@@ -1009,8 +1075,12 @@
       <c r="I17" s="8">
         <v>16.899999999999999</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J17" s="1">
+        <f t="shared" si="0"/>
+        <v>22.079175709251473</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>11</v>
       </c>
@@ -1038,8 +1108,12 @@
       <c r="I18" s="8">
         <v>18.100000000000001</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J18" s="1">
+        <f t="shared" si="0"/>
+        <v>19.675873551128554</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>11</v>
       </c>
@@ -1067,8 +1141,12 @@
       <c r="I19" s="8">
         <v>16.7</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J19" s="1">
+        <f t="shared" si="0"/>
+        <v>26.199618317830513</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>11</v>
       </c>
@@ -1096,8 +1174,12 @@
       <c r="I20" s="8">
         <v>13</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J20" s="1">
+        <f t="shared" si="0"/>
+        <v>31.092925240317935</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>11</v>
       </c>
@@ -1125,8 +1207,12 @@
       <c r="I21" s="8">
         <v>17</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J21" s="1">
+        <f t="shared" si="0"/>
+        <v>30.171841176832416</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>11</v>
       </c>
@@ -1154,8 +1240,12 @@
       <c r="I22" s="8">
         <v>6.7</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J22" s="1">
+        <f t="shared" si="0"/>
+        <v>44.149518683673101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -1174,10 +1264,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{844F1A78-C70D-8847-B2EB-3070CD299BE1}">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="J1" sqref="J1:J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1189,7 +1279,7 @@
     <col min="7" max="9" width="10.83203125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>7</v>
       </c>
@@ -1217,8 +1307,11 @@
       <c r="I1" s="9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J1" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
@@ -1246,8 +1339,12 @@
       <c r="I2" s="10">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J2" s="1">
+        <f>SQRT((D2-G2)^2+(E2-H2)^2+(F2-I2)^2)</f>
+        <v>8.6133617130595397</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>12</v>
       </c>
@@ -1275,8 +1372,12 @@
       <c r="I3" s="10">
         <v>24.1</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J3" s="1">
+        <f t="shared" ref="J3:J37" si="0">SQRT((D3-G3)^2+(E3-H3)^2+(F3-I3)^2)</f>
+        <v>2.9274562336608869</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>12</v>
       </c>
@@ -1304,8 +1405,12 @@
       <c r="I4" s="10">
         <v>20.3</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J4" s="1">
+        <f t="shared" si="0"/>
+        <v>14.90436177768105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
@@ -1333,8 +1438,12 @@
       <c r="I5" s="10">
         <v>15.9</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J5" s="1">
+        <f t="shared" si="0"/>
+        <v>23.084410323852758</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
@@ -1362,8 +1471,12 @@
       <c r="I6" s="10">
         <v>12.9</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J6" s="1">
+        <f t="shared" si="0"/>
+        <v>30.620418024579607</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
@@ -1391,8 +1504,12 @@
       <c r="I7" s="10">
         <v>16.3</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J7" s="1">
+        <f t="shared" si="0"/>
+        <v>37.196370790710205</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>12</v>
       </c>
@@ -1420,8 +1537,12 @@
       <c r="I8" s="10">
         <v>12.7</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J8" s="1">
+        <f t="shared" si="0"/>
+        <v>31.517614122899591</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>12</v>
       </c>
@@ -1449,8 +1570,12 @@
       <c r="I9" s="10">
         <v>8.6</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J9" s="1">
+        <f t="shared" si="0"/>
+        <v>39.121988702007464</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -1478,8 +1603,12 @@
       <c r="I10" s="10">
         <v>3.4</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J10" s="1">
+        <f t="shared" si="0"/>
+        <v>46.386528216713948</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>13</v>
       </c>
@@ -1507,8 +1636,12 @@
       <c r="I11" s="8">
         <v>23.8</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J11" s="1">
+        <f t="shared" si="0"/>
+        <v>1.3490737563232014</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
@@ -1536,8 +1669,12 @@
       <c r="I12" s="8">
         <v>22.4</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J12" s="1">
+        <f t="shared" si="0"/>
+        <v>3.8910152916687335</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>13</v>
       </c>
@@ -1565,8 +1702,12 @@
       <c r="I13" s="8">
         <v>22.2</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J13" s="1">
+        <f t="shared" si="0"/>
+        <v>1.9261360284258231</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>13</v>
       </c>
@@ -1594,8 +1735,12 @@
       <c r="I14" s="8">
         <v>22.3</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J14" s="1">
+        <f t="shared" si="0"/>
+        <v>12.142899159591163</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>13</v>
       </c>
@@ -1623,8 +1768,12 @@
       <c r="I15" s="8">
         <v>21.4</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J15" s="1">
+        <f t="shared" si="0"/>
+        <v>11.615076409563562</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>13</v>
       </c>
@@ -1652,8 +1801,12 @@
       <c r="I16" s="8">
         <v>19.3</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J16" s="1">
+        <f t="shared" si="0"/>
+        <v>19.661383471159901</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>13</v>
       </c>
@@ -1681,8 +1834,12 @@
       <c r="I17" s="8">
         <v>18.7</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J17" s="1">
+        <f t="shared" si="0"/>
+        <v>16.032467059064864</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>13</v>
       </c>
@@ -1710,8 +1867,12 @@
       <c r="I18" s="8">
         <v>20.6</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J18" s="1">
+        <f t="shared" si="0"/>
+        <v>9.079096871385385</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>13</v>
       </c>
@@ -1739,8 +1900,12 @@
       <c r="I19" s="8">
         <v>11.2</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J19" s="1">
+        <f t="shared" si="0"/>
+        <v>33.929633066097246</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>14</v>
       </c>
@@ -1768,8 +1933,12 @@
       <c r="I20" s="8">
         <v>21.53</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J20" s="1">
+        <f t="shared" si="0"/>
+        <v>12.751588136385211</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>14</v>
       </c>
@@ -1797,8 +1966,12 @@
       <c r="I21" s="8">
         <v>20.02</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J21" s="1">
+        <f t="shared" si="0"/>
+        <v>19.149154028311539</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>14</v>
       </c>
@@ -1826,8 +1999,12 @@
       <c r="I22" s="8">
         <v>9.4700000000000006</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J22" s="1">
+        <f t="shared" si="0"/>
+        <v>39.95212259692844</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>15</v>
       </c>
@@ -1855,8 +2032,12 @@
       <c r="I23" s="8">
         <v>19.79</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J23" s="1">
+        <f>SQRT((D23-G23)^2+(E23-H23)^2+(F23-I23)^2)</f>
+        <v>6.3308609209174698</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>15</v>
       </c>
@@ -1884,8 +2065,12 @@
       <c r="I24" s="8">
         <v>19.37</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J24" s="1">
+        <f t="shared" si="0"/>
+        <v>8.9306942619261118</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>15</v>
       </c>
@@ -1913,8 +2098,12 @@
       <c r="I25" s="8">
         <v>16.98</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J25" s="1">
+        <f t="shared" si="0"/>
+        <v>10.273349015778638</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>15</v>
       </c>
@@ -1942,8 +2131,12 @@
       <c r="I26" s="8">
         <v>21.42</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J26" s="1">
+        <f t="shared" si="0"/>
+        <v>12.174415797072156</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>15</v>
       </c>
@@ -1971,8 +2164,12 @@
       <c r="I27" s="8">
         <v>20.89</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J27" s="1">
+        <f t="shared" si="0"/>
+        <v>12.400270158347359</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>15</v>
       </c>
@@ -2000,8 +2197,12 @@
       <c r="I28" s="8">
         <v>21.22</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J28" s="1">
+        <f t="shared" si="0"/>
+        <v>18.171419867473212</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>15</v>
       </c>
@@ -2029,8 +2230,12 @@
       <c r="I29" s="8">
         <v>21.41</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J29" s="1">
+        <f t="shared" si="0"/>
+        <v>26.32718367011557</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>15</v>
       </c>
@@ -2058,8 +2263,12 @@
       <c r="I30" s="8">
         <v>22.55</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J30" s="1">
+        <f t="shared" si="0"/>
+        <v>31.077210299510472</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>15</v>
       </c>
@@ -2087,8 +2296,12 @@
       <c r="I31" s="8">
         <v>21.15</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J31" s="1">
+        <f t="shared" si="0"/>
+        <v>37.218052071541841</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>15</v>
       </c>
@@ -2116,8 +2329,12 @@
       <c r="I32" s="8">
         <v>21.89</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J32" s="1">
+        <f t="shared" si="0"/>
+        <v>23.504369806484917</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>15</v>
       </c>
@@ -2145,8 +2362,12 @@
       <c r="I33" s="8">
         <v>20.55</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J33" s="1">
+        <f t="shared" si="0"/>
+        <v>34.010671854581176</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>15</v>
       </c>
@@ -2174,8 +2395,12 @@
       <c r="I34" s="8">
         <v>20.93</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J34" s="1">
+        <f t="shared" si="0"/>
+        <v>34.142798655060481</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>15</v>
       </c>
@@ -2203,8 +2428,12 @@
       <c r="I35" s="8">
         <v>20.84</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J35" s="1">
+        <f t="shared" si="0"/>
+        <v>35.804320968285381</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>15</v>
       </c>
@@ -2232,8 +2461,12 @@
       <c r="I36" s="8">
         <v>16.89</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J36" s="1">
+        <f t="shared" si="0"/>
+        <v>35.983849154863904</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>15</v>
       </c>
@@ -2260,6 +2493,10 @@
       </c>
       <c r="I37" s="8">
         <v>18.57</v>
+      </c>
+      <c r="J37" s="1">
+        <f t="shared" si="0"/>
+        <v>40.580008624937477</v>
       </c>
     </row>
   </sheetData>
@@ -2270,10 +2507,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DE42AA7-2E73-E74B-8268-FF470DA7EEFC}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2284,7 +2521,7 @@
     <col min="4" max="9" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>7</v>
       </c>
@@ -2312,8 +2549,11 @@
       <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J1" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>16</v>
       </c>
@@ -2341,8 +2581,12 @@
       <c r="I2" s="8">
         <v>20.3</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J2" s="1">
+        <f>SQRT((D2-G2)^2+(E2-H2)^2+(F2-I2)^2)</f>
+        <v>15.681198933755034</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>16</v>
       </c>
@@ -2370,8 +2614,12 @@
       <c r="I3" s="8">
         <v>13.3</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J3" s="1">
+        <f t="shared" ref="J3" si="0">SQRT((D3-G3)^2+(E3-H3)^2+(F3-I3)^2)</f>
+        <v>27.692056622793476</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -2382,7 +2630,7 @@
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
@@ -2393,7 +2641,7 @@
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -2404,7 +2652,7 @@
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -2415,7 +2663,7 @@
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -2426,7 +2674,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -2437,7 +2685,7 @@
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -2448,7 +2696,7 @@
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -2459,7 +2707,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -2470,7 +2718,7 @@
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -2481,7 +2729,7 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -2492,7 +2740,7 @@
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
     </row>
-    <row r="15" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -2503,7 +2751,7 @@
       <c r="H15" s="8"/>
       <c r="I15" s="8"/>
     </row>
-    <row r="16" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>

</xml_diff>

<commit_message>
Jue's changes hidden layer 10->12
</commit_message>
<xml_diff>
--- a/Data4Dipesh/2hand Data_Final.xlsx
+++ b/Data4Dipesh/2hand Data_Final.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/more/Desktop/Data4Dipesh/2hand Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/more/Jue/【Python】/thermal-treatment/Data4Dipesh/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F1E367E-0F78-F640-B8BA-AE81852E70F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3AABA97-1C5E-D942-B9AB-98108C46DB45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{E91E4898-FD52-D146-A301-D679369FD159}"/>
   </bookViews>
@@ -509,7 +509,7 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F2"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>